<commit_message>
Some change. .get(begin) len(list) != real number of posts
</commit_message>
<xml_diff>
--- a/mistake.away1029.xlsx
+++ b/mistake.away1029.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Парсинг\Insta_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5232EF54-3BA2-4C58-A717-4A7B7C59A53B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2B5F27-5C0A-4695-BAA7-BBADD1FA7A39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,23 @@
     <sheet name="Locations" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Locations!$G$1:$G$819</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Locations!$G$820:$G$1029</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Locations!$G$1:$G$819</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Locations!$G$820:$G$1029</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Locations!$D$2:$D$5</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Locations!$G$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Locations!$G$2:$G$5</definedName>
+    <definedName name="_xlchart.v5.10" hidden="1">Locations!$B$1028</definedName>
+    <definedName name="_xlchart.v5.11" hidden="1">Locations!$B$1029</definedName>
+    <definedName name="_xlchart.v5.12" hidden="1">Locations!$B$1:$B$1028</definedName>
+    <definedName name="_xlchart.v5.3" hidden="1">Locations!$B$1</definedName>
+    <definedName name="_xlchart.v5.4" hidden="1">Locations!$B$2:$B$1029</definedName>
+    <definedName name="_xlchart.v5.5" hidden="1">Locations!$G$1</definedName>
+    <definedName name="_xlchart.v5.6" hidden="1">Locations!$G$2:$G$1029</definedName>
+    <definedName name="_xlchart.v5.7" hidden="1">Locations!$B$1028</definedName>
+    <definedName name="_xlchart.v5.8" hidden="1">Locations!$B$1029</definedName>
+    <definedName name="_xlchart.v5.9" hidden="1">Locations!$B$1:$B$1028</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3575,24 +3584,6 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3731,6 +3722,24 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -10723,15 +10732,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1590675</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>2305050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2676526</xdr:colOff>
+      <xdr:colOff>3390901</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>15503</xdr:rowOff>
+      <xdr:rowOff>148853</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22587,7 +22596,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DC008D24-3ACD-42AF-9C9F-911693FCBA42}" name="Сводная таблица2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DC008D24-3ACD-42AF-9C9F-911693FCBA42}" name="Сводная таблица2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -23135,7 +23144,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40CEBF2B-CCB2-483F-BC87-7340B7CCC3E8}" name="Таблица1" displayName="Таблица1" ref="A1:H1029" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40CEBF2B-CCB2-483F-BC87-7340B7CCC3E8}" name="Таблица1" displayName="Таблица1" ref="A1:H1029" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:H1029" xr:uid="{12EDE678-FC0E-49A7-9FD2-27B204999236}">
     <filterColumn colId="6">
       <filters>
@@ -23454,14 +23463,14 @@
     <sortCondition descending="1" ref="A1:A1029"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{56098E00-D392-4589-9ABC-9CC1B469FE53}" name="№" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{AAD5419B-8077-49A4-B6E2-F6B9718F12E6}" name="Location" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{D1BD2934-C820-4D32-9D0A-DAE8A7C6CC9E}" name="Site" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{DD1FF467-4E51-4D96-B016-3B33B3A505D3}" name="Date" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{5DA425E7-AA73-416C-A3EA-7E14E929534A}" name="Time" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{8E41C24F-47D1-4109-B5B1-85377846F73F}" name="Day" dataDxfId="3" dataCellStyle="data_style"/>
-    <tableColumn id="7" xr3:uid="{1253C912-117F-4ECB-B263-5A18978F8334}" name="Likes" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{1C222A80-23C9-45D1-8804-9B8CAB18E698}" name="Views" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{56098E00-D392-4589-9ABC-9CC1B469FE53}" name="№" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{AAD5419B-8077-49A4-B6E2-F6B9718F12E6}" name="Location" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{D1BD2934-C820-4D32-9D0A-DAE8A7C6CC9E}" name="Site" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{DD1FF467-4E51-4D96-B016-3B33B3A505D3}" name="Date" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{5DA425E7-AA73-416C-A3EA-7E14E929534A}" name="Time" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{8E41C24F-47D1-4109-B5B1-85377846F73F}" name="Day" dataDxfId="2" dataCellStyle="data_style"/>
+    <tableColumn id="7" xr3:uid="{1253C912-117F-4ECB-B263-5A18978F8334}" name="Likes" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{1C222A80-23C9-45D1-8804-9B8CAB18E698}" name="Views" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -26653,7 +26662,7 @@
   <dimension ref="A1:AMM1029"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>